<commit_message>
Revert "added test and fixed agents response to fit new excel format"
This reverts commit f3a78f34e80418ba624282dbf22cb7d70e39d860.
</commit_message>
<xml_diff>
--- a/CourseProposal/json_output/assessment_dataframe.xlsx
+++ b/CourseProposal/json_output/assessment_dataframe.xlsx
@@ -487,7 +487,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The candidate will describe creative principles and storytelling in AI-generated text prompts in a Written Exam.
+          <t>The candidate will answer questions on creative principles and storytelling in AI-generated text prompts to assess understanding.
 K9: Creative principles and storytelling in AI generated text prompts (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -514,7 +514,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>The candidate will explain basic AI algorithms and models used in script/text generation in a Written Exam.
+          <t>The candidate will respond to questions on basic AI algorithms and models used in script/text generation to demonstrate knowledge.
 K10: Basic AI algorithms and models used in script/text generation (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -541,7 +541,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>The candidate will incorporate unique creative principles into AI-generated story ideas in a Practical Exam.
+          <t>The candidate will incorporate unique creative principles and storytelling elements into AI-generated story ideas during a practical exam.
 A8: Incorporate unique creative principles and storytelling elements into AI-generated story ideas to avoid generic replication (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -568,7 +568,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>The candidate will use AI-generated text techniques to develop script elements in a Practical Exam.
+          <t>The candidate will use AI-generated text techniques and methodologies to develop script elements in a practical exam.
 A5: Use AI-generated text techniques and methodologies to develop script elements (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -595,7 +595,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>The candidate will respond to a series of short answer questions related to AI-generated script ideation techniques for world-building, storyline, and character development in a Written Exam.
+          <t>The candidate will respond to a series of short answer questions related to AI-generated script ideation techniques for world-building, storyline and character development, scenario iterations.
 K1: AI-generated script ideation techniques for world-building, storyline and character development, scenario iterations (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -622,7 +622,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>The candidate will identify key terms and themes for input into Gen AI platform in a Practical Exam.
+          <t>The candidate will identify key terms and themes for input into Gen AI platform to ideate and iterate story elements in a practical exam.
 A7: Identify key terms and themes for input into Gen AI platform to ideate and iterate story elements for incorporation into text prompts (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -649,7 +649,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>The candidate will explain Gen AI tool limitations and solutions in a Written Exam.
+          <t>The candidate will answer questions on Gen AI tool limitations and solutions to assess their knowledge.
 K3: Gen AI tool limitations and solutions (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -676,7 +676,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>The candidate will apply and adjust prompts in the generative process to improve iterations in a Practical Exam.
+          <t>The candidate will apply and adjust relevant prompts in the generative process to improve iterations during a practical exam.
 A6: Apply and adjust relevant prompts in the generative process to improve iterations (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -703,7 +703,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>The candidate will explain basic NLP techniques and tools relevant to AI Text generation in a Written Exam.
+          <t>The candidate will respond to questions on basic NLP techniques and tools relevant to AI text generation to demonstrate knowledge.
 K8: Basic Natural Language Processing (NLP) techniques and tools relevant to AI Text generation (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -730,7 +730,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>The candidate will utilize NLP techniques and tools to enhance AI-generated story elements in a Practical Exam.
+          <t>The candidate will utilize NLP techniques and tools to enhance the quality and effectiveness of AI-generated story elements in a practical exam.
 A2: Utilise NLP techniques and tools to enhance the quality and effectiveness of AI-generated story elements (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -757,7 +757,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>The candidate will describe AI tools for script analysis and market research in a Written Exam.
+          <t>The candidate will respond to questions about AI tools for script analysis and market research to demonstrate knowledge.
 K6: AI tools for script analysis and market research (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -784,7 +784,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>The candidate will filter and script-edit Gen-AI output in a Practical Exam.
+          <t>The candidate will filter and script-edit Gen-AI output in a practical exam to demonstrate their skills.
 A4: Filter and Script-edit Gen-AI output (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -811,7 +811,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>The candidate will discuss Gen AI and Ethics awareness in a Written Exam.
+          <t>The candidate will answer questions on Gen AI and ethics awareness to assess their understanding.
 K7: Gen AI and Ethics awareness (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -838,7 +838,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>The candidate will discuss best practices to minimize plagiarism risk in a Written Exam.
+          <t>The candidate will answer questions on best practices to minimize plagiarism risk to show understanding.
 K5: Best Practices to minimise plagiarism risk (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -865,7 +865,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>The candidate will apply ethical considerations in prompt selection and reference usage in a Practical Exam.
+          <t>The candidate will apply ethical considerations in the selection of prompts and reference usage during a practical exam.
 A3: Apply ethical considerations in the selection of prompts and reference usage (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -892,7 +892,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>The candidate will demonstrate awareness and correction of bias in LLMs training data in a Written Exam.
+          <t>The candidate will explain awareness and correction of bias in LLMs training data reproduced in output through written responses.
 K4: Awareness and correction of bias in LLMs training data reproduced in output (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -919,7 +919,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>The candidate will perform a practical exercise on analyzing AI output for bias and submit corrective steps in a Practical Exam.
+          <t>The candidate will perform a practical exercise on analyzing AI output for bias and taking corrective steps and submit their analysis.
 A1: Analyse AI output for bias and taking corrective steps (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -946,7 +946,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>The candidate will answer questions on copyright law covering Gen AI usage in a Written Exam.
+          <t>The candidate will respond to questions about copyright law covering Gen AI usage to demonstrate understanding.
 K2: Copyright law covering Gen AI usage (MED-MED-3004-1.1)</t>
         </is>
       </c>
@@ -973,7 +973,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>The candidate will identify copyright risk in Gen-AI production and avoid infringement in a Practical Exam.
+          <t>The candidate will identify copyright risk in Gen-AI production and avoid copyright infringement in a practical exam.
 A9: Identify copyright risk in Gen-AI production and avoid copyright infringement (MED-MED-3004-1.1)</t>
         </is>
       </c>

</xml_diff>